<commit_message>
Slides intro MBO + slides presentations appli
</commit_message>
<xml_diff>
--- a/TempsPerfUniversite.xlsx
+++ b/TempsPerfUniversite.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projets\perfuniversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10668"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="9156"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A30" sqref="A30:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>